<commit_message>
Update at 2025-07-23 10:31:35
</commit_message>
<xml_diff>
--- a/deep_fund.xlsx
+++ b/deep_fund.xlsx
@@ -29,6 +29,9 @@
     <t>종목</t>
   </si>
   <si>
+    <t>총점수</t>
+  </si>
+  <si>
     <t>업종</t>
   </si>
   <si>
@@ -47,9 +50,6 @@
     <t>가격/수급</t>
   </si>
   <si>
-    <t>총점수</t>
-  </si>
-  <si>
     <t>TSM</t>
   </si>
   <si>
@@ -161,11 +161,11 @@
     <t>경쟁 우위 분석</t>
   </si>
   <si>
-    <t>2025년 7월 23일 기준으로, Taiwan Semiconductor Manufacturing (TSMC)의 중장기 핵심 경쟁 우위는 다음과 같습니다:
-TSMC의 핵심 경쟁 우위는 **독보적인 첨단 미세 공정 기술 리더십**과 이를 가능하게 하는 **막대한 R&amp;D 투자 및 수십 년간 축적된 기술 노하우**에 있습니다. 이는 후발 주자가 감히 넘볼 수 없는 **경쟁 불가능한 진입 장벽**을 형성하며, AI, 고성능 컴퓨팅 등 미래 핵심 산업의 필수 파트너로서 장기적인 시장 지배력을 유지할 것입니다.</t>
-  </si>
-  <si>
-    <t>2025년 7월 23일 기준 엔비디아의 중장기 핵심 경쟁 우위는 압도적인 GPU 기술력과 이를 뒷받침하는 독점적인 CUDA 소프트웨어 플랫폼에 기반한 강력한 생태계입니다. 이는 개발자들의 높은 전환 비용과 강력한 네트워크 효과를 유발하여 AI 시대의 사실상 표준(de facto standard)으로 자리매김했으며, 타 경쟁사의 진입을 극도로 어렵게 만들어 지속적인 시장 지배력을 유지할 것입니다.</t>
+    <t>2025년 7월 23일 기준, Taiwan Semiconductor Manufacturing Company (TSMC)는 **최첨단 파운드리 기술의 압도적 리더십과 막대한 자본 투자 및 기술 노하우가 요구되는 강력한 진입 장벽**을 구축하고 있습니다. 이러한 독점적 위치는 주요 고객사들의 높은 전환 비용과 깊은 협력 관계를 통해 향후에도 유지되며, 압도적인 시장 지위와 수익성을 보장하는 핵심 요인으로 투자 가치가 높습니다.</t>
+  </si>
+  <si>
+    <t>2025년 7월 23일 기준, NVIDIA Corporation의 중장기 핵심 경쟁 우위(Moat)는 다음과 같습니다.
+NVIDIA의 중장기 핵심 경쟁 우위는 AI 가속 컴퓨팅 시장의 사실상 표준이 된 독보적인 GPU 하드웨어와 이를 기반으로 하는 독점적인 CUDA 소프트웨어 플랫폼 및 견고한 개발자 생태계입니다. 이는 타의 추종을 불허하는 높은 진입 장벽과 강력한 네트워크 효과를 창출하여 향후에도 압도적인 시장 지배력과 높은 수익성 유지를 가능하게 합니다.</t>
   </si>
   <si>
     <t>최적화 기준</t>
@@ -271,6 +271,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="$#,##0"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -300,8 +303,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -320,13 +324,13 @@
   <tableColumns count="9">
     <tableColumn id="1" name="티커"/>
     <tableColumn id="2" name="종목"/>
-    <tableColumn id="3" name="업종"/>
-    <tableColumn id="4" name="현재가"/>
-    <tableColumn id="5" name="1개월대비"/>
-    <tableColumn id="6" name="밸류에이션"/>
-    <tableColumn id="7" name="실적모멘텀"/>
-    <tableColumn id="8" name="가격/수급"/>
-    <tableColumn id="9" name="총점수"/>
+    <tableColumn id="3" name="총점수"/>
+    <tableColumn id="4" name="업종"/>
+    <tableColumn id="5" name="현재가"/>
+    <tableColumn id="6" name="1개월대비"/>
+    <tableColumn id="7" name="밸류에이션"/>
+    <tableColumn id="8" name="실적모멘텀"/>
+    <tableColumn id="9" name="가격/수급"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -718,8 +722,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
-    <col min="2" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -758,26 +763,26 @@
       <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="D2">
+      <c r="E2" s="1">
         <v>234.6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>34</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>100</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>97</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>67</v>
-      </c>
-      <c r="I2">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -787,26 +792,26 @@
       <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="D3">
+      <c r="E3" s="1">
         <v>167.03</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>35</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>24</v>
-      </c>
-      <c r="G3">
-        <v>100</v>
       </c>
       <c r="H3">
         <v>100</v>
       </c>
       <c r="I3">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -816,26 +821,26 @@
       <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
         <v>29</v>
       </c>
-      <c r="D4">
+      <c r="E4" s="1">
         <v>505.27</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>36</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>25</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>87</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>50</v>
-      </c>
-      <c r="I4">
-        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -845,26 +850,26 @@
       <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
         <v>30</v>
       </c>
-      <c r="D5">
+      <c r="E5" s="1">
         <v>192.11</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>37</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>44</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>41</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>75</v>
-      </c>
-      <c r="I5">
-        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -874,26 +879,26 @@
       <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="D6">
+      <c r="E6" s="1">
         <v>191.34</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>38</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>37</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>41</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>75</v>
-      </c>
-      <c r="I6">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -903,26 +908,26 @@
       <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
         <v>31</v>
       </c>
-      <c r="D7">
+      <c r="E7" s="1">
         <v>227.47</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>39</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>9</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>51</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>83</v>
-      </c>
-      <c r="I7">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -932,26 +937,26 @@
       <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8">
+        <v>47</v>
+      </c>
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="D8">
+      <c r="E8" s="1">
         <v>704.8099999999999</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>40</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>19</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>89</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>33</v>
-      </c>
-      <c r="I8">
-        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -961,26 +966,26 @@
       <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
         <v>32</v>
       </c>
-      <c r="D9">
+      <c r="E9" s="1">
         <v>332.11</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>41</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>28</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>9</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>83</v>
-      </c>
-      <c r="I9">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -990,26 +995,26 @@
       <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="D10">
+      <c r="E10" s="1">
         <v>278.59</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>42</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
         <v>67</v>
-      </c>
-      <c r="I10">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1019,30 +1024,30 @@
       <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
         <v>33</v>
       </c>
-      <c r="D11">
+      <c r="E11" s="1">
         <v>214.4</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>43</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>11</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>44</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>0</v>
       </c>
-      <c r="I11">
-        <v>18</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I1:I11">
+  <conditionalFormatting sqref="C1:C11">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1074,26 +1079,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1498,102 +1503,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>0.2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>0.03</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>0.4</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>0.18</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>